<commit_message>
project works for adding queue items
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Platon\HRobot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347B450B-1EF6-43E6-9C80-BCEDF6A1ABEE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801F60AB-144D-41F7-BA68-BE7CC983567C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>cristiHRobot-mailAccount</t>
+  </si>
+  <si>
+    <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
 </sst>
 </file>
@@ -524,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -581,7 +590,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2797,8 +2816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Config added folder name in GoogleDrive
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Platon\HRobot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9857BDB-684C-4EF8-8E81-11DB448D3107}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583B9D48-F3DF-42FC-AFA5-05BDDDAFB247}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
   </si>
   <si>
-    <t>Cristi-Hrobot</t>
-  </si>
-  <si>
     <t>outlookAccount</t>
   </si>
   <si>
@@ -187,6 +184,15 @@
   </si>
   <si>
     <t>googleAccount</t>
+  </si>
+  <si>
+    <t>GoogleDriveFolderName</t>
+  </si>
+  <si>
+    <t>HRobot</t>
+  </si>
+  <si>
+    <t>Cristi-HRobot</t>
   </si>
 </sst>
 </file>
@@ -559,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -610,7 +616,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -618,13 +624,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1630,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1860,11 +1866,11 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>53</v>
+      <c r="B25" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2853,7 +2859,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2897,21 +2903,28 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>